<commit_message>
New commissioned portraits, new animations
</commit_message>
<xml_diff>
--- a/Documents/Character List.xlsx
+++ b/Documents/Character List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugob\BindingStories\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008BAFFF-941B-425E-A89A-B8967AEA1961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA990EF-2E41-4808-83F9-1A5EBED8C77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="403">
   <si>
     <t>Name</t>
   </si>
@@ -216,15 +216,9 @@
     <t>Talk with any Lord or Céleste.</t>
   </si>
   <si>
-    <t>Sarin</t>
-  </si>
-  <si>
     <t>0x0E</t>
   </si>
   <si>
-    <t>Sword Cavalier 4</t>
-  </si>
-  <si>
     <t>Talk with Apatheia.</t>
   </si>
   <si>
@@ -330,9 +324,6 @@
     <t>Game Over Unit on its joining chapter, including as an enemy.</t>
   </si>
   <si>
-    <t>Torm</t>
-  </si>
-  <si>
     <t>0x1D</t>
   </si>
   <si>
@@ -369,18 +360,9 @@
     <t>Myrmidon 7</t>
   </si>
   <si>
-    <t>Umbra</t>
-  </si>
-  <si>
     <t>0x4E</t>
   </si>
   <si>
-    <t>Free from her cell, then talk with any Lord.</t>
-  </si>
-  <si>
-    <t>Charlie</t>
-  </si>
-  <si>
     <t>0x43</t>
   </si>
   <si>
@@ -444,15 +426,9 @@
     <t>Axe Armor 7</t>
   </si>
   <si>
-    <t>Roswenn</t>
-  </si>
-  <si>
     <t>0x24</t>
   </si>
   <si>
-    <t>Nomad 8</t>
-  </si>
-  <si>
     <t>Felrindel</t>
   </si>
   <si>
@@ -471,15 +447,9 @@
     <t>Sword General 1</t>
   </si>
   <si>
-    <t>Laurine</t>
-  </si>
-  <si>
     <t>0x40</t>
   </si>
   <si>
-    <t>Troubadour 12</t>
-  </si>
-  <si>
     <t>Nandil</t>
   </si>
   <si>
@@ -522,9 +492,6 @@
     <t>Mage 3</t>
   </si>
   <si>
-    <t>Ruby</t>
-  </si>
-  <si>
     <t>0x2A</t>
   </si>
   <si>
@@ -621,9 +588,6 @@
     <t>0x2F</t>
   </si>
   <si>
-    <t>Nomad Trooper 1</t>
-  </si>
-  <si>
     <t>Eilfinia</t>
   </si>
   <si>
@@ -633,9 +597,6 @@
     <t>Light Mage ?</t>
   </si>
   <si>
-    <t>Viktor</t>
-  </si>
-  <si>
     <t>0x3F</t>
   </si>
   <si>
@@ -648,9 +609,6 @@
     <t>Bors</t>
   </si>
   <si>
-    <t>Vincent</t>
-  </si>
-  <si>
     <t>0x2B</t>
   </si>
   <si>
@@ -687,15 +645,9 @@
     <t>Makes an appearance in Prologue.</t>
   </si>
   <si>
-    <t>Ismena</t>
-  </si>
-  <si>
     <t>0x6A</t>
   </si>
   <si>
-    <t>Falcoknight 5</t>
-  </si>
-  <si>
     <t>Jacob</t>
   </si>
   <si>
@@ -774,9 +726,6 @@
     <t>0x55</t>
   </si>
   <si>
-    <t>↑ Celindra comes back</t>
-  </si>
-  <si>
     <t>Queen 5</t>
   </si>
   <si>
@@ -798,12 +747,6 @@
     <t>Falcoknight ?</t>
   </si>
   <si>
-    <t>Limstella</t>
-  </si>
-  <si>
-    <t>Nino</t>
-  </si>
-  <si>
     <t>0x3C</t>
   </si>
   <si>
@@ -894,18 +837,12 @@
     <t>Mage 7</t>
   </si>
   <si>
-    <t>Arturo</t>
-  </si>
-  <si>
     <t>0x2D</t>
   </si>
   <si>
     <t>Hero 2</t>
   </si>
   <si>
-    <t>Talk with Mevrick.</t>
-  </si>
-  <si>
     <t>Frank</t>
   </si>
   <si>
@@ -927,328 +864,376 @@
     <t>Talk with Nailda.</t>
   </si>
   <si>
-    <t>Sheryl</t>
+    <t>0x38</t>
+  </si>
+  <si>
+    <t>0x3D</t>
+  </si>
+  <si>
+    <t>Dies at some point during the story.</t>
+  </si>
+  <si>
+    <t>Nailda</t>
+  </si>
+  <si>
+    <t>0x47</t>
+  </si>
+  <si>
+    <t>Dancer 1</t>
+  </si>
+  <si>
+    <t>Mandatory to recruit Aldrina.</t>
+  </si>
+  <si>
+    <t>0x4C</t>
+  </si>
+  <si>
+    <t>0x4F</t>
+  </si>
+  <si>
+    <t>Eliot</t>
+  </si>
+  <si>
+    <t>0x52</t>
+  </si>
+  <si>
+    <t>Fighter 15</t>
+  </si>
+  <si>
+    <t>Talk with Laura, Artémisia or Lisri.</t>
+  </si>
+  <si>
+    <t>Ascelline</t>
+  </si>
+  <si>
+    <t>0x56</t>
+  </si>
+  <si>
+    <t>Acolyte ?</t>
+  </si>
+  <si>
+    <t>Sora</t>
+  </si>
+  <si>
+    <t>0x58</t>
+  </si>
+  <si>
+    <t>Mage Armor 8</t>
+  </si>
+  <si>
+    <t>Talk with Sham or any Lord.</t>
+  </si>
+  <si>
+    <t>Grain</t>
+  </si>
+  <si>
+    <t>0x5C</t>
+  </si>
+  <si>
+    <t>Wyvern Rider 8</t>
+  </si>
+  <si>
+    <t>Manfred</t>
+  </si>
+  <si>
+    <t>0x5E</t>
+  </si>
+  <si>
+    <t>Jasmine</t>
+  </si>
+  <si>
+    <t>0x5F</t>
+  </si>
+  <si>
+    <t>Thief 6</t>
+  </si>
+  <si>
+    <t>Alaïs</t>
+  </si>
+  <si>
+    <t>Talk with Alesia or any Lord.</t>
+  </si>
+  <si>
+    <t>0x66</t>
+  </si>
+  <si>
+    <t>Cleric 7</t>
+  </si>
+  <si>
+    <t>Galgaliel</t>
+  </si>
+  <si>
+    <t>0x67</t>
+  </si>
+  <si>
+    <t>Reyzana</t>
+  </si>
+  <si>
+    <t>0x6B</t>
+  </si>
+  <si>
+    <t>Talk with any Lord, Guinivere, Bardulphus, Galgaliel, Manfred or Jasmine.</t>
+  </si>
+  <si>
+    <t>Wyvern Rider 3</t>
+  </si>
+  <si>
+    <t>Hime</t>
+  </si>
+  <si>
+    <t>0x6C</t>
+  </si>
+  <si>
+    <t>Automatically recruited during the second part of the map.</t>
+  </si>
+  <si>
+    <t>0x6D</t>
+  </si>
+  <si>
+    <t>Krilalaris</t>
+  </si>
+  <si>
+    <t>Archer ?</t>
+  </si>
+  <si>
+    <t>Free from her cell and pay 50 gold.</t>
+  </si>
+  <si>
+    <t>Adaleide</t>
+  </si>
+  <si>
+    <t>0x6F</t>
+  </si>
+  <si>
+    <t>Bishop ?</t>
+  </si>
+  <si>
+    <t>Amïsty</t>
+  </si>
+  <si>
+    <t>0x72</t>
+  </si>
+  <si>
+    <t>Talk and defeat in battle with either Laura, Artémisia or Lisri.</t>
+  </si>
+  <si>
+    <t>Andriet</t>
+  </si>
+  <si>
+    <t>0x5D</t>
+  </si>
+  <si>
+    <t>Hero 15</t>
+  </si>
+  <si>
+    <t>Pandora</t>
+  </si>
+  <si>
+    <t>Defeat Borvir with Pandora.</t>
+  </si>
+  <si>
+    <t>Ellie</t>
+  </si>
+  <si>
+    <t>0x59</t>
+  </si>
+  <si>
+    <t>Shaman 2</t>
+  </si>
+  <si>
+    <t>Swordmaster 2</t>
+  </si>
+  <si>
+    <t>Alte</t>
+  </si>
+  <si>
+    <t>0x57</t>
+  </si>
+  <si>
+    <t>Visit village, then Talk with any Lord.</t>
+  </si>
+  <si>
+    <t>Kae</t>
+  </si>
+  <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>Myrmidon 14</t>
+  </si>
+  <si>
+    <t>Sylvio</t>
+  </si>
+  <si>
+    <t>0x22</t>
+  </si>
+  <si>
+    <t>Reika / Star Breaker</t>
+  </si>
+  <si>
+    <t>Saki</t>
+  </si>
+  <si>
+    <t>0x3E</t>
+  </si>
+  <si>
+    <t>Thief 3</t>
+  </si>
+  <si>
+    <t>Talk with any Lord or Brad, Céleste.</t>
+  </si>
+  <si>
+    <t>Sumika</t>
+  </si>
+  <si>
+    <t>0x41</t>
+  </si>
+  <si>
+    <t>Poppo</t>
+  </si>
+  <si>
+    <t>0x42</t>
+  </si>
+  <si>
+    <t>Joins after some doors are opened.</t>
+  </si>
+  <si>
+    <t>Free from her cell, then talk with any Lord or Cecilia.</t>
+  </si>
+  <si>
+    <t>NoName</t>
+  </si>
+  <si>
+    <t>0x45</t>
+  </si>
+  <si>
+    <t>Joins on Turn 1, if spared last chapter.</t>
+  </si>
+  <si>
+    <t>Mira</t>
+  </si>
+  <si>
+    <t>0x48</t>
+  </si>
+  <si>
+    <t>Assassin ?</t>
+  </si>
+  <si>
+    <t>Malt</t>
+  </si>
+  <si>
+    <t>0x4D</t>
+  </si>
+  <si>
+    <t>Mage Knight ?</t>
+  </si>
+  <si>
+    <t>Pass Malt's trials, then recruit him at the end of the chapter.</t>
+  </si>
+  <si>
+    <t>Defeat in battle six times, then recruit her at the end of the chapter.</t>
+  </si>
+  <si>
+    <t>Axe General 3</t>
+  </si>
+  <si>
+    <t>Fernet</t>
+  </si>
+  <si>
+    <t>Troubadour 4</t>
+  </si>
+  <si>
+    <t>Nanako</t>
+  </si>
+  <si>
+    <t>Syura</t>
+  </si>
+  <si>
+    <t>Islay</t>
+  </si>
+  <si>
+    <t>Kai</t>
+  </si>
+  <si>
+    <t>Bourbon</t>
+  </si>
+  <si>
+    <t>Sherry</t>
+  </si>
+  <si>
+    <t>Marc</t>
   </si>
   <si>
     <t>0x37</t>
   </si>
   <si>
-    <t>Soldier 10</t>
-  </si>
-  <si>
-    <t>Shiroyasha</t>
-  </si>
-  <si>
-    <t>0x38</t>
-  </si>
-  <si>
-    <t>Berserker ?</t>
-  </si>
-  <si>
-    <t>Ellyn</t>
-  </si>
-  <si>
-    <t>0x3D</t>
-  </si>
-  <si>
-    <t>Cleric 1</t>
-  </si>
-  <si>
-    <t>Dies at some point during the story.</t>
-  </si>
-  <si>
-    <t>Nailda</t>
-  </si>
-  <si>
-    <t>0x47</t>
-  </si>
-  <si>
-    <t>Dancer 1</t>
-  </si>
-  <si>
-    <t>Mandatory to recruit Aldrina.</t>
-  </si>
-  <si>
-    <t>0x4C</t>
-  </si>
-  <si>
-    <t>0x4F</t>
-  </si>
-  <si>
-    <t>Eliot</t>
-  </si>
-  <si>
-    <t>0x52</t>
-  </si>
-  <si>
-    <t>Fighter 15</t>
-  </si>
-  <si>
-    <t>Talk with Laura, Artémisia or Lisri.</t>
-  </si>
-  <si>
-    <t>Ascelline</t>
-  </si>
-  <si>
-    <t>0x56</t>
-  </si>
-  <si>
-    <t>Acolyte ?</t>
-  </si>
-  <si>
-    <t>Valkyrie ?</t>
-  </si>
-  <si>
-    <t>Sora</t>
-  </si>
-  <si>
-    <t>0x58</t>
-  </si>
-  <si>
-    <t>Mage Armor 8</t>
-  </si>
-  <si>
-    <t>Talk with Sham or any Lord.</t>
-  </si>
-  <si>
-    <t>Grain</t>
-  </si>
-  <si>
-    <t>0x5C</t>
-  </si>
-  <si>
-    <t>Wyvern Rider 8</t>
-  </si>
-  <si>
-    <t>Manfred</t>
-  </si>
-  <si>
-    <t>0x5E</t>
-  </si>
-  <si>
-    <t>Jasmine</t>
-  </si>
-  <si>
-    <t>0x5F</t>
-  </si>
-  <si>
-    <t>Thief 6</t>
-  </si>
-  <si>
-    <t>Alaïs</t>
-  </si>
-  <si>
-    <t>Talk with Alesia or any Lord.</t>
-  </si>
-  <si>
-    <t>0x66</t>
-  </si>
-  <si>
-    <t>Cleric 7</t>
-  </si>
-  <si>
-    <t>Galgaliel</t>
-  </si>
-  <si>
-    <t>0x67</t>
-  </si>
-  <si>
-    <t>Clarine</t>
+    <t>Sword Cavalier 3</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Sweet Breaker</t>
+  </si>
+  <si>
+    <t>Rozette</t>
+  </si>
+  <si>
+    <t>Cleric 12</t>
+  </si>
+  <si>
+    <t>Tsih</t>
+  </si>
+  <si>
+    <t>Noa</t>
+  </si>
+  <si>
+    <t>Ilscea</t>
+  </si>
+  <si>
+    <t>Archéa</t>
+  </si>
+  <si>
+    <t>Suguri (46B)</t>
+  </si>
+  <si>
+    <t>Swordmaster 5</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Mercenary ?</t>
+  </si>
+  <si>
+    <t>Archer 8</t>
+  </si>
+  <si>
+    <t>Scholar ?</t>
+  </si>
+  <si>
+    <t>Armless</t>
+  </si>
+  <si>
+    <t>Sagi</t>
+  </si>
+  <si>
+    <t>Yselle</t>
+  </si>
+  <si>
+    <t>0x6E</t>
   </si>
   <si>
     <t>0x68</t>
   </si>
   <si>
-    <t>Klein</t>
-  </si>
-  <si>
     <t>0x69</t>
   </si>
   <si>
-    <t>Sniper ?</t>
-  </si>
-  <si>
-    <t>Reyzana</t>
-  </si>
-  <si>
-    <t>0x6B</t>
-  </si>
-  <si>
-    <t>Warrior ?</t>
-  </si>
-  <si>
-    <t>Talk with any Lord, Guinivere, Bardulphus, Galgaliel, Manfred or Jasmine.</t>
-  </si>
-  <si>
-    <t>Wyvern Rider 3</t>
-  </si>
-  <si>
-    <t>Hime</t>
-  </si>
-  <si>
-    <t>0x6C</t>
-  </si>
-  <si>
-    <t>Automatically recruited during the second part of the map.</t>
-  </si>
-  <si>
-    <t>Marcus</t>
-  </si>
-  <si>
-    <t>0x6D</t>
-  </si>
-  <si>
-    <t>Lance Paladin ?</t>
-  </si>
-  <si>
-    <t>Krilalaris</t>
-  </si>
-  <si>
-    <t>Archer ?</t>
-  </si>
-  <si>
-    <t>Free from her cell and pay 50 gold.</t>
-  </si>
-  <si>
-    <t>Adaleide</t>
-  </si>
-  <si>
-    <t>0x6F</t>
-  </si>
-  <si>
-    <t>Bishop ?</t>
-  </si>
-  <si>
-    <t>Amïsty</t>
-  </si>
-  <si>
-    <t>0x72</t>
-  </si>
-  <si>
-    <t>Talk and defeat in battle with either Laura, Artémisia or Lisri.</t>
-  </si>
-  <si>
-    <t>Andriet</t>
-  </si>
-  <si>
-    <t>0x5D</t>
-  </si>
-  <si>
-    <t>Hero 15</t>
-  </si>
-  <si>
-    <t>Pandora</t>
-  </si>
-  <si>
-    <t>Defeat Borvir with Pandora.</t>
-  </si>
-  <si>
-    <t>Ellie</t>
-  </si>
-  <si>
-    <t>0x59</t>
-  </si>
-  <si>
-    <t>Shaman 2</t>
-  </si>
-  <si>
-    <t>Swordmaster 2</t>
-  </si>
-  <si>
-    <t>Alte</t>
-  </si>
-  <si>
-    <t>0x57</t>
-  </si>
-  <si>
-    <t>Visit village, then Talk with any Lord.</t>
-  </si>
-  <si>
-    <t>Kae</t>
-  </si>
-  <si>
-    <t>0x11</t>
-  </si>
-  <si>
-    <t>Myrmidon 14</t>
-  </si>
-  <si>
-    <t>Sylvio</t>
-  </si>
-  <si>
-    <t>0x22</t>
-  </si>
-  <si>
-    <t>Reika / Star Breaker</t>
-  </si>
-  <si>
-    <t>Saki</t>
-  </si>
-  <si>
-    <t>0x3E</t>
-  </si>
-  <si>
-    <t>Thief 3</t>
-  </si>
-  <si>
-    <t>Talk with any Lord or Brad, Céleste.</t>
-  </si>
-  <si>
-    <t>Sumika</t>
-  </si>
-  <si>
-    <t>0x41</t>
-  </si>
-  <si>
-    <t>Poppo</t>
-  </si>
-  <si>
-    <t>0x42</t>
-  </si>
-  <si>
-    <t>Open the chest she's hiding in to recruit.</t>
-  </si>
-  <si>
-    <t>Joins after some doors are opened.</t>
-  </si>
-  <si>
-    <t>Free from her cell, then talk with any Lord or Cecilia.</t>
-  </si>
-  <si>
-    <t>NoName</t>
-  </si>
-  <si>
-    <t>0x45</t>
-  </si>
-  <si>
-    <t>Axe General ?</t>
-  </si>
-  <si>
-    <t>Joins on Turn 1, if spared last chapter.</t>
-  </si>
-  <si>
-    <t>Mira</t>
-  </si>
-  <si>
-    <t>0x48</t>
-  </si>
-  <si>
-    <t>Assassin ?</t>
-  </si>
-  <si>
-    <t>Malt</t>
-  </si>
-  <si>
-    <t>0x4D</t>
-  </si>
-  <si>
-    <t>Mage Knight ?</t>
-  </si>
-  <si>
-    <t>Pass Malt's trials, then recruit him at the end of the chapter.</t>
-  </si>
-  <si>
-    <t>Defeat in battle six times, then recruit her at the end of the chapter.</t>
+    <t>Fighter 4</t>
+  </si>
+  <si>
+    <t>Pegasus Knight 12</t>
   </si>
 </sst>
 </file>
@@ -1580,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G156"/>
+  <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1756,7 +1741,7 @@
         <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1802,21 +1787,21 @@
         <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>11</v>
@@ -1876,16 +1861,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>11</v>
@@ -1922,16 +1907,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>340</v>
+        <v>311</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>341</v>
+        <v>312</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>351</v>
+        <v>316</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>41</v>
@@ -1945,16 +1930,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>382</v>
+        <v>345</v>
       </c>
       <c r="B19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>11</v>
@@ -1968,16 +1953,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="B21" s="1">
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>11</v>
@@ -2003,7 +1988,7 @@
         <v>55</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>57</v>
@@ -2026,7 +2011,7 @@
         <v>61</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>62</v>
@@ -2037,22 +2022,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>370</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>371</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>26</v>
@@ -2060,197 +2045,200 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>385</v>
+        <v>348</v>
       </c>
       <c r="B25" s="1">
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>386</v>
+        <v>349</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>387</v>
+        <v>350</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="1">
-        <v>5</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B28" s="1">
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B29" s="1">
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>352</v>
+        <v>79</v>
       </c>
       <c r="B30" s="1">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>353</v>
+        <v>80</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B31" s="1">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="1">
-        <v>6</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B35" s="1">
         <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>104</v>
+        <v>372</v>
       </c>
       <c r="B36" s="1">
         <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>11</v>
@@ -2264,16 +2252,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>306</v>
+        <v>101</v>
       </c>
       <c r="B37" s="1">
         <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>307</v>
+        <v>102</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>308</v>
+        <v>104</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>11</v>
@@ -2282,96 +2270,96 @@
         <v>12</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="1">
-        <v>7</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B38" s="1">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="B40" s="1">
         <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>279</v>
+        <v>108</v>
       </c>
       <c r="B41" s="1">
         <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>280</v>
+        <v>109</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>281</v>
+        <v>110</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>395</v>
+        <v>12</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>333</v>
+        <v>260</v>
       </c>
       <c r="B42" s="1">
         <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>334</v>
+        <v>261</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>335</v>
+        <v>262</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>394</v>
+        <v>357</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>26</v>
@@ -2379,22 +2367,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>114</v>
+        <v>304</v>
       </c>
       <c r="B43" s="1">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>115</v>
+        <v>305</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>106</v>
+        <v>306</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>116</v>
+        <v>356</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>26</v>
@@ -2402,22 +2390,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="B44" s="1">
         <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>26</v>
@@ -2425,22 +2413,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>117</v>
+        <v>385</v>
       </c>
       <c r="B45" s="1">
         <v>7</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>26</v>
@@ -2448,36 +2436,36 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>391</v>
+        <v>354</v>
       </c>
       <c r="B46" s="1">
         <v>7</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>392</v>
+        <v>355</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>393</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B48" s="1">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>11</v>
@@ -2491,16 +2479,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B49" s="1">
         <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>11</v>
@@ -2514,16 +2502,16 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B50" s="1">
         <v>8</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>11</v>
@@ -2537,16 +2525,16 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B52" s="1">
         <v>9</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>11</v>
@@ -2560,16 +2548,16 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B53" s="1">
         <v>9</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>11</v>
@@ -2583,22 +2571,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="B54" s="1">
         <v>9</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>337</v>
+        <v>308</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>26</v>
@@ -2606,22 +2594,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>336</v>
+        <v>307</v>
       </c>
       <c r="B55" s="1">
         <v>9</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>338</v>
+        <v>309</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>339</v>
+        <v>310</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>337</v>
+        <v>308</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>26</v>
@@ -2629,16 +2617,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B57" s="1">
         <v>10</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>11</v>
@@ -2652,16 +2640,16 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>139</v>
+        <v>373</v>
       </c>
       <c r="B58" s="1">
         <v>10</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>141</v>
+        <v>393</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>11</v>
@@ -2675,16 +2663,16 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B59" s="1">
         <v>10</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>11</v>
@@ -2698,16 +2686,16 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B60" s="1">
         <v>10</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>56</v>
@@ -2721,16 +2709,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
       <c r="B61" s="1">
         <v>10</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>329</v>
+        <v>300</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>330</v>
+        <v>301</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>56</v>
@@ -2744,16 +2732,16 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B63" s="1">
         <v>11</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>11</v>
@@ -2767,108 +2755,85 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>151</v>
+        <v>295</v>
       </c>
       <c r="B64" s="1">
         <v>11</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>152</v>
+        <v>296</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>153</v>
+        <v>297</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>12</v>
+        <v>298</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B65" s="1">
-        <v>11</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G65" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="B66" s="1">
-        <v>11</v>
+        <v>144</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>325</v>
+        <v>145</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>326</v>
+        <v>146</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>327</v>
+        <v>12</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>159</v>
+        <v>377</v>
+      </c>
+      <c r="B69" s="1">
+        <v>13</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>11</v>
@@ -2877,21 +2842,44 @@
         <v>12</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B70" s="1">
+        <v>13</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B71" s="1">
         <v>13</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>11</v>
@@ -2905,108 +2893,108 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>185</v>
+        <v>253</v>
       </c>
       <c r="B72" s="1">
         <v>13</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>186</v>
+        <v>254</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>205</v>
+        <v>159</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>168</v>
+        <v>339</v>
       </c>
       <c r="B73" s="1">
         <v>13</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>169</v>
+        <v>340</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>170</v>
+        <v>25</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>12</v>
+        <v>341</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B74" s="1">
-        <v>13</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>376</v>
+        <v>160</v>
       </c>
       <c r="B75" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>377</v>
+        <v>287</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>378</v>
+        <v>12</v>
       </c>
       <c r="G75" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B76" s="1">
+        <v>14</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B77" s="1">
         <v>14</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>315</v>
+        <v>165</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>11</v>
@@ -3020,16 +3008,16 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B78" s="1">
         <v>14</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>11</v>
@@ -3038,90 +3026,90 @@
         <v>12</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>175</v>
+        <v>327</v>
       </c>
       <c r="B79" s="1">
         <v>14</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>176</v>
+        <v>328</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>177</v>
+        <v>117</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>12</v>
+        <v>329</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B80" s="1">
-        <v>14</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>364</v>
+        <v>182</v>
       </c>
       <c r="B81" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>365</v>
+        <v>183</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>123</v>
+        <v>184</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>366</v>
+        <v>26</v>
       </c>
       <c r="G81" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B82" s="1">
+        <v>15</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B83" s="1">
         <v>15</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>26</v>
@@ -3135,16 +3123,16 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>196</v>
+        <v>397</v>
       </c>
       <c r="B84" s="1">
         <v>15</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>197</v>
+        <v>280</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>198</v>
+        <v>402</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>26</v>
@@ -3153,44 +3141,21 @@
         <v>26</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B85" s="1">
-        <v>15</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G85" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>342</v>
+        <v>167</v>
       </c>
       <c r="B86" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>343</v>
+        <v>168</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>323</v>
+        <v>169</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>26</v>
@@ -3204,16 +3169,16 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>344</v>
+        <v>179</v>
       </c>
       <c r="B87" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>345</v>
+        <v>180</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>346</v>
+        <v>181</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>26</v>
@@ -3223,20 +3188,43 @@
       </c>
       <c r="G87" s="1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B88" s="1">
+        <v>16</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>178</v>
+        <v>292</v>
       </c>
       <c r="B89" s="1">
         <v>16</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>179</v>
+        <v>293</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>180</v>
+        <v>294</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>26</v>
@@ -3250,154 +3238,128 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>190</v>
+        <v>352</v>
       </c>
       <c r="B90" s="1">
         <v>16</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>191</v>
+        <v>353</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>310</v>
+        <v>358</v>
       </c>
       <c r="B91" s="1">
         <v>16</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>311</v>
+        <v>359</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B92" s="1">
-        <v>16</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>26</v>
+        <v>360</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="B93" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>390</v>
+        <v>190</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>260</v>
+        <v>191</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
       <c r="B94" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>397</v>
+        <v>270</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>398</v>
+        <v>271</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B96" s="1">
+        <v>26</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B95" s="1">
         <v>17</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G96" s="1" t="s">
+      <c r="C95" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>289</v>
+        <v>193</v>
       </c>
       <c r="B97" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>290</v>
+        <v>194</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>291</v>
+        <v>195</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>292</v>
+        <v>26</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>26</v>
@@ -3405,42 +3367,68 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>400</v>
+        <v>288</v>
       </c>
       <c r="B98" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>401</v>
+        <v>289</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>402</v>
+        <v>290</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>26</v>
+        <v>291</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B99" s="1">
+        <v>18</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>206</v>
+        <v>383</v>
       </c>
       <c r="B100" s="1">
         <v>18</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>208</v>
+        <v>140</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>209</v>
+        <v>384</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>26</v>
@@ -3448,65 +3436,65 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="B101" s="1">
         <v>18</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>317</v>
+        <v>343</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>318</v>
+        <v>344</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>319</v>
+        <v>12</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="B102" s="1">
-        <v>18</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G102" s="1" t="s">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B103" s="1">
+        <v>19</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>210</v>
+        <v>333</v>
       </c>
       <c r="B104" s="1">
         <v>19</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>211</v>
+        <v>286</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>212</v>
+        <v>337</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>12</v>
@@ -3517,16 +3505,16 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>370</v>
+        <v>335</v>
       </c>
       <c r="B105" s="1">
         <v>19</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>314</v>
+        <v>336</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>374</v>
+        <v>338</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>11</v>
@@ -3540,22 +3528,22 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>372</v>
+        <v>176</v>
       </c>
       <c r="B106" s="1">
         <v>19</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>373</v>
+        <v>177</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>375</v>
+        <v>178</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>12</v>
+        <v>334</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>26</v>
@@ -3563,130 +3551,130 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>187</v>
+        <v>321</v>
       </c>
       <c r="B107" s="1">
         <v>19</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>188</v>
+        <v>398</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>189</v>
+        <v>322</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>371</v>
+        <v>323</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B108" s="1">
-        <v>19</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>26</v>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B109" s="1">
+        <v>20</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="B110" s="1">
         <v>20</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>260</v>
+        <v>366</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="B111" s="1">
-        <v>20</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>406</v>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B112" s="1">
+        <v>21</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B113" s="1">
-        <v>21</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>26</v>
+      <c r="F113" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F114" s="2" t="s">
-        <v>233</v>
+      <c r="A114" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B114" s="1">
+        <v>22</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>216</v>
+        <v>389</v>
       </c>
       <c r="B115" s="1">
         <v>22</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>218</v>
+        <v>390</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>26</v>
@@ -3695,49 +3683,49 @@
         <v>26</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>219</v>
+        <v>26</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B116" s="1">
-        <v>22</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>26</v>
+      <c r="F116" s="2" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F117" s="2" t="s">
-        <v>232</v>
+      <c r="A117" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B117" s="1">
+        <v>23</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B118" s="1">
         <v>23</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>11</v>
@@ -3746,21 +3734,21 @@
         <v>12</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>219</v>
+        <v>26</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B119" s="1">
         <v>23</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>11</v>
@@ -3772,47 +3760,47 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B120" s="1">
-        <v>23</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G120" s="1" t="s">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B121" s="1">
+        <v>24</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>207</v>
+        <v>272</v>
       </c>
       <c r="B122" s="1">
         <v>24</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>235</v>
+        <v>274</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>26</v>
@@ -3820,22 +3808,22 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>293</v>
+        <v>220</v>
       </c>
       <c r="B123" s="1">
         <v>24</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>294</v>
+        <v>221</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>295</v>
+        <v>222</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>26</v>
@@ -3843,22 +3831,22 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B124" s="1">
         <v>24</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>26</v>
+        <v>226</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>26</v>
@@ -3866,44 +3854,39 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>239</v>
+        <v>386</v>
       </c>
       <c r="B125" s="1">
         <v>24</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>240</v>
+        <v>111</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>241</v>
+        <v>103</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>242</v>
+        <v>26</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F126" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>11</v>
@@ -3917,16 +3900,16 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B129" s="1">
         <v>25</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>26</v>
@@ -3940,16 +3923,16 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>331</v>
+        <v>302</v>
       </c>
       <c r="B130" s="1">
         <v>25</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>26</v>
@@ -3963,16 +3946,16 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="B132" s="1">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>26</v>
@@ -3986,22 +3969,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>347</v>
+        <v>313</v>
       </c>
       <c r="B133" s="1">
         <v>26</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>348</v>
+        <v>314</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>349</v>
+        <v>394</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>26</v>
@@ -4009,16 +3992,16 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="B135" s="1">
         <v>27</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>26</v>
@@ -4032,16 +4015,16 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>361</v>
+        <v>324</v>
       </c>
       <c r="B137" s="1">
         <v>28</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>362</v>
+        <v>325</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>363</v>
+        <v>326</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>26</v>
@@ -4055,16 +4038,16 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="B139" s="1">
         <v>29</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>26</v>
@@ -4078,16 +4061,16 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>367</v>
+        <v>330</v>
       </c>
       <c r="B140" s="1">
         <v>29</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>368</v>
+        <v>331</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>26</v>
@@ -4101,16 +4084,16 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>258</v>
+        <v>395</v>
       </c>
       <c r="B142" s="1">
         <v>30</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>26</v>
@@ -4122,151 +4105,117 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A143" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B143" s="1">
-        <v>30</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A145" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E145" s="1" t="s">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E144" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F145" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A147" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B147" s="1">
+      <c r="F144" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B146" s="1">
         <v>31</v>
       </c>
-      <c r="C147" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G147" s="1" t="s">
+      <c r="C146" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G146" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>303</v>
+        <v>243</v>
       </c>
       <c r="B148" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>304</v>
+        <v>244</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>305</v>
+        <v>239</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>26</v>
+        <v>246</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>26</v>
+        <v>245</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B150" s="1">
-        <v>32</v>
+        <v>387</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G150" s="1" t="s">
-        <v>264</v>
+        <v>400</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>388</v>
+      </c>
       <c r="B152" s="1" t="s">
-        <v>266</v>
+        <v>248</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
+        <v>250</v>
+      </c>
       <c r="B154" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G156" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G154" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Paladin/Troubadour animations, added Marc and Fernet portraits
</commit_message>
<xml_diff>
--- a/Documents/Character List.xlsx
+++ b/Documents/Character List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugob\BindingStories\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE58F4BC-6466-407A-A7A7-A4742064FEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49739CBB-DA1A-424C-99FF-7474B89F1074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1567,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3425,13 +3425,13 @@
         <v>383</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>11</v>
+        <v>380</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>12</v>
+        <v>380</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>26</v>
+        <v>380</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
New track and documentation update
</commit_message>
<xml_diff>
--- a/Documents/Character List.xlsx
+++ b/Documents/Character List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugob\BindingStories\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49739CBB-DA1A-424C-99FF-7474B89F1074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EF5D10-7C93-4367-AE88-7A2179153B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1128,9 +1128,6 @@
     <t>Pass Malt's trials, then recruit him at the end of the chapter.</t>
   </si>
   <si>
-    <t>Defeat in battle six times, then recruit her at the end of the chapter.</t>
-  </si>
-  <si>
     <t>Axe General 3</t>
   </si>
   <si>
@@ -1234,6 +1231,9 @@
   </si>
   <si>
     <t>Reach the second part of the map with any Lord.</t>
+  </si>
+  <si>
+    <t>Defeat in battle five times, then recruit her at the end of the chapter.</t>
   </si>
 </sst>
 </file>
@@ -1567,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="G98" sqref="G98"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
@@ -2031,7 +2031,7 @@
         <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>41</v>
@@ -2068,22 +2068,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B26" s="1">
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>26</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B36" s="1">
         <v>6</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B38" s="1">
         <v>6</v>
@@ -2284,7 +2284,7 @@
         <v>240</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>11</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B45" s="1">
         <v>7</v>
@@ -2640,7 +2640,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B58" s="1">
         <v>10</v>
@@ -2649,7 +2649,7 @@
         <v>133</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>11</v>
@@ -2824,7 +2824,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B69" s="1">
         <v>13</v>
@@ -3123,7 +3123,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B84" s="1">
         <v>15</v>
@@ -3132,7 +3132,7 @@
         <v>279</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>26</v>
@@ -3267,7 +3267,7 @@
         <v>358</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>11</v>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B93" s="1">
         <v>17</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B94" s="1">
         <v>17</v>
@@ -3390,7 +3390,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B99" s="1">
         <v>18</v>
@@ -3399,21 +3399,21 @@
         <v>319</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B100" s="1">
         <v>18</v>
@@ -3422,16 +3422,16 @@
         <v>140</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -3557,7 +3557,7 @@
         <v>19</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>321</v>
@@ -3589,7 +3589,7 @@
         <v>41</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>367</v>
+        <v>402</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
@@ -3665,7 +3665,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B115" s="1">
         <v>22</v>
@@ -3674,7 +3674,7 @@
         <v>206</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>26</v>
@@ -3762,7 +3762,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B121" s="1">
         <v>24</v>
@@ -3854,7 +3854,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B125" s="1">
         <v>24</v>
@@ -3978,7 +3978,7 @@
         <v>313</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>56</v>
@@ -4084,7 +4084,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B142" s="1">
         <v>30</v>
@@ -4093,7 +4093,7 @@
         <v>242</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>26</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B145" s="1">
         <v>31</v>
@@ -4176,24 +4176,24 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>247</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
File management & new assets
</commit_message>
<xml_diff>
--- a/Documents/Character List.xlsx
+++ b/Documents/Character List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugob\BindingStories\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EF5D10-7C93-4367-AE88-7A2179153B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7148971-687D-4169-A91C-E31A3ECCD098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="402">
   <si>
     <t>Name</t>
   </si>
@@ -675,12 +675,6 @@
     <t>Mage Knight 5</t>
   </si>
   <si>
-    <t>↨ Celindra dies</t>
-  </si>
-  <si>
-    <t>Melchior joins for 2 chapters</t>
-  </si>
-  <si>
     <t>0x2C</t>
   </si>
   <si>
@@ -906,9 +900,6 @@
     <t>0x56</t>
   </si>
   <si>
-    <t>Acolyte ?</t>
-  </si>
-  <si>
     <t>Sora</t>
   </si>
   <si>
@@ -1107,15 +1098,9 @@
     <t>Joins on Turn 1, if spared last chapter.</t>
   </si>
   <si>
-    <t>Mira</t>
-  </si>
-  <si>
     <t>0x48</t>
   </si>
   <si>
-    <t>Assassin ?</t>
-  </si>
-  <si>
     <t>Malt</t>
   </si>
   <si>
@@ -1234,6 +1219,18 @@
   </si>
   <si>
     <t>Defeat in battle five times, then recruit her at the end of the chapter.</t>
+  </si>
+  <si>
+    <t>Druid ?</t>
+  </si>
+  <si>
+    <t>Celindra dies, Melchior joins for 2 chapters</t>
+  </si>
+  <si>
+    <t>Assassin 1</t>
+  </si>
+  <si>
+    <t>Terra</t>
   </si>
 </sst>
 </file>
@@ -1567,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1907,16 +1904,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>41</v>
@@ -1930,7 +1927,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
@@ -1953,13 +1950,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B21" s="1">
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>154</v>
@@ -2022,7 +2019,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
@@ -2031,7 +2028,7 @@
         <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>41</v>
@@ -2045,22 +2042,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B25" s="1">
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>26</v>
@@ -2068,22 +2065,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B26" s="1">
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>26</v>
@@ -2160,13 +2157,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B31" s="1">
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>88</v>
@@ -2175,7 +2172,7 @@
         <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>26</v>
@@ -2229,7 +2226,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B36" s="1">
         <v>6</v>
@@ -2275,16 +2272,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B38" s="1">
         <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>11</v>
@@ -2293,7 +2290,7 @@
         <v>12</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2344,22 +2341,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B42" s="1">
         <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>26</v>
@@ -2367,22 +2364,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B43" s="1">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>26</v>
@@ -2390,22 +2387,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B44" s="1">
         <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>26</v>
@@ -2413,7 +2410,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B45" s="1">
         <v>7</v>
@@ -2436,16 +2433,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B46" s="1">
         <v>7</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>11</v>
@@ -2571,22 +2568,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B54" s="1">
         <v>9</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>26</v>
@@ -2594,22 +2591,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B55" s="1">
         <v>9</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>26</v>
@@ -2640,7 +2637,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B58" s="1">
         <v>10</v>
@@ -2649,7 +2646,7 @@
         <v>133</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>11</v>
@@ -2709,16 +2706,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B61" s="1">
         <v>10</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>56</v>
@@ -2730,87 +2727,84 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B63" s="1">
-        <v>11</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="1" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B62" s="1">
+        <v>10</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="1">
+        <v>11</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B65" s="1">
+        <v>11</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B64" s="1">
-        <v>11</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>58</v>
+      <c r="G65" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>11</v>
@@ -2822,44 +2816,44 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B69" s="1">
-        <v>13</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>26</v>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>174</v>
+        <v>370</v>
       </c>
       <c r="B70" s="1">
         <v>13</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>192</v>
+        <v>156</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>12</v>
@@ -2870,19 +2864,19 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B71" s="1">
         <v>13</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>12</v>
@@ -2893,13 +2887,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>253</v>
+        <v>157</v>
       </c>
       <c r="B72" s="1">
         <v>13</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>254</v>
+        <v>158</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>159</v>
@@ -2911,67 +2905,67 @@
         <v>12</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>338</v>
+        <v>251</v>
       </c>
       <c r="B73" s="1">
         <v>13</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>339</v>
+        <v>252</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B74" s="1">
+        <v>13</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B75" s="1">
-        <v>14</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G75" s="1" t="s">
+      <c r="F74" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B76" s="1">
         <v>14</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>163</v>
+        <v>284</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>11</v>
@@ -2985,16 +2979,16 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B77" s="1">
         <v>14</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>166</v>
+        <v>71</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>11</v>
@@ -3008,16 +3002,16 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B78" s="1">
         <v>14</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>11</v>
@@ -3026,67 +3020,67 @@
         <v>12</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>173</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>326</v>
+        <v>170</v>
       </c>
       <c r="B79" s="1">
         <v>14</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>327</v>
+        <v>171</v>
       </c>
       <c r="D79" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B80" s="1">
+        <v>14</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E80" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B81" s="1">
-        <v>15</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G81" s="1" t="s">
+      <c r="F80" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G80" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B82" s="1">
         <v>15</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>26</v>
@@ -3100,16 +3094,16 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B83" s="1">
         <v>15</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>189</v>
+        <v>71</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>26</v>
@@ -3123,16 +3117,16 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>395</v>
+        <v>187</v>
       </c>
       <c r="B84" s="1">
         <v>15</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>279</v>
+        <v>188</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>400</v>
+        <v>189</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>26</v>
@@ -3144,41 +3138,41 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B86" s="1">
-        <v>16</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G86" s="1" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B85" s="1">
+        <v>15</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G85" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B87" s="1">
         <v>16</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>26</v>
@@ -3192,16 +3186,16 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>281</v>
+        <v>179</v>
       </c>
       <c r="B88" s="1">
         <v>16</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>282</v>
+        <v>180</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>283</v>
+        <v>181</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>26</v>
@@ -3210,21 +3204,21 @@
         <v>26</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>284</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="B89" s="1">
         <v>16</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>26</v>
@@ -3233,84 +3227,84 @@
         <v>26</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>26</v>
+        <v>282</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>351</v>
+        <v>289</v>
       </c>
       <c r="B90" s="1">
         <v>16</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>143</v>
+        <v>398</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="B91" s="1">
         <v>16</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>367</v>
+        <v>143</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B93" s="1">
-        <v>17</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B92" s="1">
+        <v>16</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B94" s="1">
         <v>17</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>270</v>
+        <v>190</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>271</v>
+        <v>191</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>26</v>
@@ -3324,21 +3318,24 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="B95" s="1">
         <v>17</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>361</v>
+        <v>268</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>362</v>
+        <v>269</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3367,22 +3364,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B98" s="1">
         <v>18</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>26</v>
@@ -3390,30 +3387,30 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B99" s="1">
         <v>18</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B100" s="1">
         <v>18</v>
@@ -3422,30 +3419,30 @@
         <v>140</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B101" s="1">
         <v>18</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>11</v>
@@ -3482,16 +3479,16 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B104" s="1">
         <v>19</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>11</v>
@@ -3505,16 +3502,16 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B105" s="1">
         <v>19</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>11</v>
@@ -3543,7 +3540,7 @@
         <v>26</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>26</v>
@@ -3551,22 +3548,22 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B107" s="1">
         <v>19</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>26</v>
@@ -3574,42 +3571,42 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B109" s="1">
         <v>20</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B110" s="1">
         <v>20</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -3637,7 +3634,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F113" s="2" t="s">
-        <v>217</v>
+        <v>399</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -3665,7 +3662,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B115" s="1">
         <v>22</v>
@@ -3674,7 +3671,7 @@
         <v>206</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>26</v>
@@ -3687,9 +3684,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F116" s="2" t="s">
-        <v>216</v>
-      </c>
+      <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
@@ -3762,16 +3757,16 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B121" s="1">
         <v>24</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>26</v>
@@ -3785,16 +3780,16 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B122" s="1">
         <v>24</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>11</v>
@@ -3808,16 +3803,16 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B123" s="1">
         <v>24</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>26</v>
@@ -3831,22 +3826,22 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B124" s="1">
         <v>24</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>26</v>
@@ -3854,7 +3849,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B125" s="1">
         <v>24</v>
@@ -3877,16 +3872,16 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="D127" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>11</v>
@@ -3900,16 +3895,16 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B129" s="1">
         <v>25</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>26</v>
@@ -3923,16 +3918,16 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B130" s="1">
         <v>25</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>26</v>
@@ -3946,16 +3941,16 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B132" s="1">
+        <v>26</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="B132" s="1">
-        <v>26</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>26</v>
@@ -3969,22 +3964,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B133" s="1">
         <v>26</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>26</v>
@@ -3992,16 +3987,16 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B135" s="1">
         <v>27</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>26</v>
@@ -4015,16 +4010,16 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B137" s="1">
         <v>28</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>26</v>
@@ -4038,16 +4033,16 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B139" s="1">
         <v>29</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>26</v>
@@ -4061,16 +4056,16 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B140" s="1">
         <v>29</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>26</v>
@@ -4084,16 +4079,16 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B142" s="1">
         <v>30</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>26</v>
@@ -4107,22 +4102,22 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B143" s="1">
         <v>30</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>26</v>
@@ -4130,16 +4125,16 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B145" s="1">
         <v>31</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>26</v>
@@ -4153,61 +4148,61 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B147" s="1">
         <v>32</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
New portraits and saves (2)
</commit_message>
<xml_diff>
--- a/Documents/Character List.xlsx
+++ b/Documents/Character List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugob\BindingStories\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7148971-687D-4169-A91C-E31A3ECCD098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E25FB28-BA85-43C9-AA0C-B7D57783C01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="405">
   <si>
     <t>Name</t>
   </si>
@@ -1026,9 +1026,6 @@
     <t>0x59</t>
   </si>
   <si>
-    <t>Shaman 2</t>
-  </si>
-  <si>
     <t>Swordmaster 2</t>
   </si>
   <si>
@@ -1107,9 +1104,6 @@
     <t>0x4D</t>
   </si>
   <si>
-    <t>Mage Knight ?</t>
-  </si>
-  <si>
     <t>Pass Malt's trials, then recruit him at the end of the chapter.</t>
   </si>
   <si>
@@ -1231,6 +1225,21 @@
   </si>
   <si>
     <t>Terra</t>
+  </si>
+  <si>
+    <t>Sage 10</t>
+  </si>
+  <si>
+    <t>Wyvern Lord 10</t>
+  </si>
+  <si>
+    <t>Estelle</t>
+  </si>
+  <si>
+    <t>Sniper 4</t>
+  </si>
+  <si>
+    <t>Druid 2</t>
   </si>
 </sst>
 </file>
@@ -1562,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G153"/>
+  <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1927,7 +1936,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
@@ -2019,7 +2028,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
@@ -2028,7 +2037,7 @@
         <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>41</v>
@@ -2042,22 +2051,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B25" s="1">
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>26</v>
@@ -2065,22 +2074,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B26" s="1">
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>26</v>
@@ -2226,7 +2235,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B36" s="1">
         <v>6</v>
@@ -2272,7 +2281,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B38" s="1">
         <v>6</v>
@@ -2281,7 +2290,7 @@
         <v>238</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>11</v>
@@ -2356,7 +2365,7 @@
         <v>56</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>26</v>
@@ -2379,7 +2388,7 @@
         <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>26</v>
@@ -2410,7 +2419,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B45" s="1">
         <v>7</v>
@@ -2433,13 +2442,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B46" s="1">
         <v>7</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>223</v>
@@ -2637,7 +2646,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B58" s="1">
         <v>10</v>
@@ -2646,7 +2655,7 @@
         <v>133</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>11</v>
@@ -2729,16 +2738,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B62" s="1">
         <v>10</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>56</v>
@@ -2841,7 +2850,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B70" s="1">
         <v>13</v>
@@ -2933,13 +2942,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B74" s="1">
         <v>13</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>25</v>
@@ -2948,7 +2957,7 @@
         <v>41</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>26</v>
@@ -3140,7 +3149,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B85" s="1">
         <v>15</v>
@@ -3149,7 +3158,7 @@
         <v>277</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>26</v>
@@ -3241,7 +3250,7 @@
         <v>290</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>26</v>
@@ -3255,13 +3264,13 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B91" s="1">
         <v>16</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>143</v>
@@ -3275,27 +3284,27 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B92" s="1">
         <v>16</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B94" s="1">
         <v>17</v>
@@ -3318,7 +3327,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B95" s="1">
         <v>17</v>
@@ -3387,7 +3396,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B99" s="1">
         <v>18</v>
@@ -3396,21 +3405,21 @@
         <v>316</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B100" s="1">
         <v>18</v>
@@ -3419,30 +3428,30 @@
         <v>140</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B101" s="1">
         <v>18</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>11</v>
@@ -3488,7 +3497,7 @@
         <v>283</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>333</v>
+        <v>404</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>11</v>
@@ -3511,7 +3520,7 @@
         <v>332</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>11</v>
@@ -3554,7 +3563,7 @@
         <v>19</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>318</v>
@@ -3569,158 +3578,158 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="B109" s="1">
-        <v>20</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>397</v>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B108" s="1">
+        <v>19</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="B110" s="1">
         <v>20</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>360</v>
+        <v>400</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B111" s="1">
+        <v>20</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B113" s="1">
         <v>21</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F113" s="2" t="s">
-        <v>399</v>
+      <c r="E113" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B114" s="1">
-        <v>22</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>205</v>
+      <c r="F114" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>382</v>
+        <v>202</v>
       </c>
       <c r="B115" s="1">
         <v>22</v>
       </c>
       <c r="C115" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B116" s="1">
+        <v>22</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F116" s="2"/>
+      <c r="D116" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B117" s="1">
-        <v>23</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>205</v>
-      </c>
+      <c r="F117" s="2"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B118" s="1">
         <v>23</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>11</v>
@@ -3729,73 +3738,73 @@
         <v>12</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>26</v>
+        <v>205</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B119" s="1">
         <v>23</v>
       </c>
       <c r="C119" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B120" s="1">
+        <v>23</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B121" s="1">
-        <v>24</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G121" s="1" t="s">
+      <c r="E120" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G120" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>270</v>
+        <v>367</v>
       </c>
       <c r="B122" s="1">
         <v>24</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>271</v>
+        <v>216</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>272</v>
+        <v>217</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>26</v>
@@ -3803,22 +3812,22 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>218</v>
+        <v>270</v>
       </c>
       <c r="B123" s="1">
         <v>24</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>26</v>
@@ -3826,22 +3835,22 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B124" s="1">
         <v>24</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>224</v>
+        <v>26</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>26</v>
@@ -3849,368 +3858,391 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>379</v>
+        <v>221</v>
       </c>
       <c r="B125" s="1">
         <v>24</v>
       </c>
       <c r="C125" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B126" s="1">
+        <v>24</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E125" s="1" t="s">
+      <c r="E126" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F125" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
+      <c r="F126" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B128" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C128" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B129" s="1">
-        <v>25</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G129" s="1" t="s">
+      <c r="E128" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G128" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>298</v>
+        <v>229</v>
       </c>
       <c r="B130" s="1">
         <v>25</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B131" s="1">
+        <v>25</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="E130" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G130" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B132" s="1">
-        <v>26</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G132" s="1" t="s">
+      <c r="E131" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G131" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B133" s="1">
+        <v>26</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B133" s="1">
-        <v>26</v>
-      </c>
-      <c r="C133" s="1" t="s">
+      <c r="B134" s="1">
+        <v>26</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="D133" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="E133" s="1" t="s">
+      <c r="D134" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E134" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F133" s="1" t="s">
+      <c r="F134" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G133" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
+      <c r="G134" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B135" s="1">
+      <c r="B136" s="1">
         <v>27</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="D136" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E135" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
+      <c r="E136" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B138" s="1">
         <v>28</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D138" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E137" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A139" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B139" s="1">
-        <v>29</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>37</v>
+      <c r="E138" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>326</v>
+        <v>235</v>
       </c>
       <c r="B140" s="1">
         <v>29</v>
       </c>
       <c r="C140" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B141" s="1">
+        <v>29</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="D141" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E140" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A142" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="B142" s="1">
-        <v>30</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G142" s="1" t="s">
+      <c r="E141" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G141" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>273</v>
+        <v>386</v>
       </c>
       <c r="B143" s="1">
         <v>30</v>
       </c>
       <c r="C143" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B144" s="1">
+        <v>30</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="D144" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E143" s="1" t="s">
+      <c r="E144" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F143" s="1" t="s">
+      <c r="F144" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G143" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A145" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B145" s="1">
+      <c r="G144" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B146" s="1">
         <v>31</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E145" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A147" s="1" t="s">
+      <c r="E146" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B147" s="1">
+      <c r="B148" s="1">
         <v>32</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C148" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="D148" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E147" s="1" t="s">
+      <c r="E148" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F147" s="1" t="s">
+      <c r="F148" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="G147" s="1" t="s">
+      <c r="G148" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A149" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B149" s="1" t="s">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C149" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A151" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B151" s="1" t="s">
+      <c r="C150" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C151" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A153" s="1" t="s">
+      <c r="C152" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B154" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C154" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D153" s="1" t="s">
+      <c r="D154" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E153" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G153" s="1" t="s">
+      <c r="E154" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G154" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>